<commit_message>
Update health and education estimates
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8DBE5D-ED47-4208-AABC-2C6C5543D603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17859ACA-0498-49C8-9D40-CFB684BACB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="11115" windowHeight="20985" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -44,12 +44,6 @@
     <t>COEFFICIENT</t>
   </si>
   <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
     <t>Constant</t>
   </si>
   <si>
@@ -140,7 +134,46 @@
     <t>REGRESSORS</t>
   </si>
   <si>
-    <t>CAT</t>
+    <t>Dgn_Low</t>
+  </si>
+  <si>
+    <t>Dag_Low</t>
+  </si>
+  <si>
+    <t>Dag_sq_Low</t>
+  </si>
+  <si>
+    <t>HUA_Low</t>
+  </si>
+  <si>
+    <t>HUB_Low</t>
+  </si>
+  <si>
+    <t>Year_transformed_Low</t>
+  </si>
+  <si>
+    <t>Constant_Low</t>
+  </si>
+  <si>
+    <t>Dgn_Medium</t>
+  </si>
+  <si>
+    <t>Dag_Medium</t>
+  </si>
+  <si>
+    <t>Dag_sq_Medium</t>
+  </si>
+  <si>
+    <t>HUA_Medium</t>
+  </si>
+  <si>
+    <t>HUB_Medium</t>
+  </si>
+  <si>
+    <t>Year_transformed_Medium</t>
+  </si>
+  <si>
+    <t>Constant_Medium</t>
   </si>
 </sst>
 </file>
@@ -544,66 +577,66 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -627,36 +660,36 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5">
         <v>-8.3379256292782949E-2</v>
@@ -685,7 +718,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5">
         <v>-0.44382673821451712</v>
@@ -714,7 +747,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>7.2106130008844291E-3</v>
@@ -743,7 +776,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B5" s="5">
         <v>-0.14725229771664056</v>
@@ -772,7 +805,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
         <v>-0.25614167040955504</v>
@@ -801,7 +834,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5">
         <v>-3.6298093281369015E-2</v>
@@ -830,7 +863,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B8" s="5">
         <v>7.7741883368231361</v>
@@ -884,45 +917,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="N1" s="4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="5">
         <v>-1.1268101667649291E-2</v>
@@ -966,7 +999,7 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="5">
         <v>-0.63039659758565159</v>
@@ -1010,7 +1043,7 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>9.1327993641878713E-3</v>
@@ -1054,7 +1087,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5">
         <v>0.20548480534059291</v>
@@ -1098,7 +1131,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" s="5">
         <v>-0.78735759097626878</v>
@@ -1142,7 +1175,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="5">
         <v>0.72368505280927786</v>
@@ -1186,7 +1219,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="5">
         <v>-9.8977204724184822E-2</v>
@@ -1230,7 +1263,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="5">
         <v>-0.40535348629865831</v>
@@ -1274,7 +1307,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B10" s="5">
         <v>7.5541391245292244E-2</v>
@@ -1318,7 +1351,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" s="5">
         <v>-7.9563105100996137E-2</v>
@@ -1362,7 +1395,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" s="5">
         <v>4.6914795306990699E-3</v>
@@ -1406,7 +1439,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B13" s="5">
         <v>7.9111055450213721</v>
@@ -1455,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4166C8A3-8125-479C-A99A-1257D5F59E53}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1464,845 +1497,753 @@
     <col min="1" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="F1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.41379566713805094</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.8006708482058549E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-1.0413845165261629E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2.7761471073766179E-4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>-2.6026573684412492E-4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-1.2017738306277469E-3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1.7834668652452445E-4</v>
+      </c>
+      <c r="I2" s="4">
+        <v>8.5711575329947665E-2</v>
+      </c>
+      <c r="J2" s="4">
+        <v>5.4643406357876264E-4</v>
+      </c>
+      <c r="K2" s="4">
+        <v>1.9305934574519595E-3</v>
+      </c>
+      <c r="L2" s="4">
+        <v>-3.9215826092171553E-5</v>
+      </c>
+      <c r="M2" s="4">
+        <v>-2.602657368440803E-4</v>
+      </c>
+      <c r="N2" s="4">
+        <v>-1.2017738306277972E-3</v>
+      </c>
+      <c r="O2" s="4">
+        <v>-5.8053821501349986E-6</v>
+      </c>
+      <c r="P2" s="4">
+        <v>-2.3068567761102582E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2.5342748337312027</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-1.0413845165261629E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.44461993036470349</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-1.0648507729289675E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-1.6876698489636213E-3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5.6554129175876867E-3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3.1801245536059559E-4</v>
+      </c>
+      <c r="I3" s="4">
+        <v>-4.6134665027390236</v>
+      </c>
+      <c r="J3" s="4">
+        <v>9.9585808110615875E-4</v>
+      </c>
+      <c r="K3" s="4">
+        <v>-1.5547597491159387E-2</v>
+      </c>
+      <c r="L3" s="4">
+        <v>3.0601582871698542E-4</v>
+      </c>
+      <c r="M3" s="4">
+        <v>-1.6876698489273244E-3</v>
+      </c>
+      <c r="N3" s="4">
+        <v>5.6554129175789957E-3</v>
+      </c>
+      <c r="O3" s="4">
+        <v>9.9158329431915139E-5</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0.19039686679488499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.41379566713805094</v>
-      </c>
-      <c r="D3" s="4">
-        <v>1.8006708482058549E-2</v>
-      </c>
-      <c r="E3" s="4">
-        <v>-1.0413845165261629E-2</v>
-      </c>
-      <c r="F3" s="4">
+      <c r="B4" s="5">
+        <v>-3.5462932151367588E-2</v>
+      </c>
+      <c r="C4" s="4">
         <v>2.7761471073766179E-4</v>
       </c>
-      <c r="G3" s="4">
+      <c r="D4" s="4">
+        <v>-1.0648507729289675E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.5624364995984031E-4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3.5708259359456035E-5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-1.2925818533043081E-4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-3.342489340852493E-6</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.1099138401010646</v>
+      </c>
+      <c r="J4" s="4">
+        <v>-2.6320624719421192E-5</v>
+      </c>
+      <c r="K4" s="4">
+        <v>3.8713232302430619E-4</v>
+      </c>
+      <c r="L4" s="4">
+        <v>-7.643592462939163E-6</v>
+      </c>
+      <c r="M4" s="4">
+        <v>3.5708259358577926E-5</v>
+      </c>
+      <c r="N4" s="4">
+        <v>-1.292581853302221E-4</v>
+      </c>
+      <c r="O4" s="4">
+        <v>-2.2230649277966551E-6</v>
+      </c>
+      <c r="P4" s="4">
+        <v>-4.7312092617540491E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3.963015435313573E-2</v>
+      </c>
+      <c r="C5" s="4">
         <v>-2.6026573684412492E-4</v>
       </c>
-      <c r="H3" s="4">
+      <c r="D5" s="4">
+        <v>-1.6876698489636213E-3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3.5708259359456035E-5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.6695229473375381E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.8051536760197905E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-1.3805572918502144E-4</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3.1667958915616943E-3</v>
+      </c>
+      <c r="J5" s="4">
+        <v>4.0361149902828821E-4</v>
+      </c>
+      <c r="K5" s="4">
+        <v>2.7228022868254521E-3</v>
+      </c>
+      <c r="L5" s="4">
+        <v>-4.6969842548320233E-5</v>
+      </c>
+      <c r="M5" s="4">
+        <v>2.6695229473375229E-2</v>
+      </c>
+      <c r="N5" s="4">
+        <v>1.8051536760197929E-2</v>
+      </c>
+      <c r="O5" s="4">
+        <v>3.6997136432840932E-4</v>
+      </c>
+      <c r="P5" s="4">
+        <v>-6.1308688662759236E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.2816127840512892</v>
+      </c>
+      <c r="C6" s="4">
         <v>-1.2017738306277469E-3</v>
       </c>
-      <c r="I3" s="4">
+      <c r="D6" s="4">
+        <v>5.6554129175876867E-3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-1.2925818533043081E-4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.8051536760197905E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.2470661711412248E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-1.3296445028694755E-4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-7.7059339860899495E-2</v>
+      </c>
+      <c r="J6" s="4">
+        <v>4.1308486621342085E-4</v>
+      </c>
+      <c r="K6" s="4">
+        <v>-8.0466931606505872E-4</v>
+      </c>
+      <c r="L6" s="4">
+        <v>2.6110918848061635E-5</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1.8051536760197988E-2</v>
+      </c>
+      <c r="N6" s="4">
+        <v>2.2470661711412227E-2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2.7717215468628929E-4</v>
+      </c>
+      <c r="P6" s="4">
+        <v>-1.7778852112508667E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-3.7910917136234706E-3</v>
+      </c>
+      <c r="C7" s="4">
         <v>1.7834668652452445E-4</v>
       </c>
-      <c r="J3" s="4">
+      <c r="D7" s="4">
+        <v>3.1801245536059559E-4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-3.342489340852493E-6</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-1.3805572918502144E-4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-1.3296445028694755E-4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6.0044282389084039E-4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>-1.3794018318166575E-2</v>
+      </c>
+      <c r="J7" s="4">
+        <v>4.222582879213118E-6</v>
+      </c>
+      <c r="K7" s="4">
+        <v>8.5420470336085731E-5</v>
+      </c>
+      <c r="L7" s="4">
+        <v>-1.8808789396120872E-6</v>
+      </c>
+      <c r="M7" s="4">
+        <v>-1.380557291850026E-4</v>
+      </c>
+      <c r="N7" s="4">
+        <v>-1.3296445028696763E-4</v>
+      </c>
+      <c r="O7" s="4">
+        <v>2.3038586009592921E-5</v>
+      </c>
+      <c r="P7" s="4">
+        <v>-1.1738908394724051E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-36.440248401675419</v>
+      </c>
+      <c r="C8" s="4">
         <v>8.5711575329947665E-2</v>
       </c>
-      <c r="K3" s="4">
+      <c r="D8" s="4">
+        <v>-4.6134665027390236</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.1099138401010646</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.1667958915616943E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-7.7059339860899495E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-1.3794018318166575E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>48.290712115621027</v>
+      </c>
+      <c r="J8" s="4">
+        <v>-1.0116274927731983E-2</v>
+      </c>
+      <c r="K8" s="4">
+        <v>0.1512957316426764</v>
+      </c>
+      <c r="L8" s="4">
+        <v>-2.972868257114937E-3</v>
+      </c>
+      <c r="M8" s="4">
+        <v>3.1667958914687253E-3</v>
+      </c>
+      <c r="N8" s="4">
+        <v>-7.7059339860927334E-2</v>
+      </c>
+      <c r="O8" s="4">
+        <v>-1.6822763833527488E-3</v>
+      </c>
+      <c r="P8" s="4">
+        <v>-1.83006133806348</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="5">
+        <v>-0.72516532133752731</v>
+      </c>
+      <c r="C9" s="4">
         <v>5.4643406357876264E-4</v>
       </c>
-      <c r="L3" s="4">
+      <c r="D9" s="4">
+        <v>9.9585808110615875E-4</v>
+      </c>
+      <c r="E9" s="4">
+        <v>-2.6320624719421192E-5</v>
+      </c>
+      <c r="F9" s="4">
+        <v>4.0361149902828821E-4</v>
+      </c>
+      <c r="G9" s="4">
+        <v>4.1308486621342085E-4</v>
+      </c>
+      <c r="H9" s="4">
+        <v>4.222582879213118E-6</v>
+      </c>
+      <c r="I9" s="4">
+        <v>-1.0116274927731983E-2</v>
+      </c>
+      <c r="J9" s="4">
+        <v>2.0866752686068551E-2</v>
+      </c>
+      <c r="K9" s="4">
+        <v>6.1764252112221363E-3</v>
+      </c>
+      <c r="L9" s="4">
+        <v>-1.3628547951569179E-4</v>
+      </c>
+      <c r="M9" s="4">
+        <v>4.0361149902829667E-4</v>
+      </c>
+      <c r="N9" s="4">
+        <v>4.1308486621334322E-4</v>
+      </c>
+      <c r="O9" s="4">
+        <v>6.4916357692590757E-5</v>
+      </c>
+      <c r="P9" s="4">
+        <v>-8.0116635570056771E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="5">
+        <v>6.905081187492188</v>
+      </c>
+      <c r="C10" s="4">
         <v>1.9305934574519595E-3</v>
       </c>
-      <c r="M3" s="4">
+      <c r="D10" s="4">
+        <v>-1.5547597491159387E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3.8713232302430619E-4</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2.7228022868254521E-3</v>
+      </c>
+      <c r="G10" s="4">
+        <v>-8.0466931606505872E-4</v>
+      </c>
+      <c r="H10" s="4">
+        <v>8.5420470336085731E-5</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.1512957316426764</v>
+      </c>
+      <c r="J10" s="4">
+        <v>6.1764252112221363E-3</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.98565093511474089</v>
+      </c>
+      <c r="L10" s="4">
+        <v>-2.0477000205447154E-2</v>
+      </c>
+      <c r="M10" s="4">
+        <v>2.7228022868038548E-3</v>
+      </c>
+      <c r="N10" s="4">
+        <v>-8.0466931609579628E-4</v>
+      </c>
+      <c r="O10" s="4">
+        <v>-1.375334198365108E-3</v>
+      </c>
+      <c r="P10" s="4">
+        <v>-11.789704530453577</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="5">
+        <v>-0.12868226744750794</v>
+      </c>
+      <c r="C11" s="4">
         <v>-3.9215826092171553E-5</v>
       </c>
-      <c r="N3" s="4">
+      <c r="D11" s="4">
+        <v>3.0601582871698542E-4</v>
+      </c>
+      <c r="E11" s="4">
+        <v>-7.643592462939163E-6</v>
+      </c>
+      <c r="F11" s="4">
+        <v>-4.6969842548320233E-5</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2.6110918848061635E-5</v>
+      </c>
+      <c r="H11" s="4">
+        <v>-1.8808789396120872E-6</v>
+      </c>
+      <c r="I11" s="4">
+        <v>-2.972868257114937E-3</v>
+      </c>
+      <c r="J11" s="4">
+        <v>-1.3628547951569179E-4</v>
+      </c>
+      <c r="K11" s="4">
+        <v>-2.0477000205447154E-2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>4.2629215885812023E-4</v>
+      </c>
+      <c r="M11" s="4">
+        <v>-4.6969842548117216E-5</v>
+      </c>
+      <c r="N11" s="4">
+        <v>2.61109188486831E-5</v>
+      </c>
+      <c r="O11" s="4">
+        <v>2.2307345343262723E-5</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0.2445039237348734</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="5">
+        <v>3.9630154353135744E-2</v>
+      </c>
+      <c r="C12" s="4">
         <v>-2.602657368440803E-4</v>
       </c>
-      <c r="O3" s="4">
+      <c r="D12" s="4">
+        <v>-1.6876698489273244E-3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>3.5708259358577926E-5</v>
+      </c>
+      <c r="F12" s="4">
+        <v>2.6695229473375229E-2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.8051536760197988E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>-1.380557291850026E-4</v>
+      </c>
+      <c r="I12" s="4">
+        <v>3.1667958914687253E-3</v>
+      </c>
+      <c r="J12" s="4">
+        <v>4.0361149902829667E-4</v>
+      </c>
+      <c r="K12" s="4">
+        <v>2.7228022868038548E-3</v>
+      </c>
+      <c r="L12" s="4">
+        <v>-4.6969842548117216E-5</v>
+      </c>
+      <c r="M12" s="4">
+        <v>2.6695229473375232E-2</v>
+      </c>
+      <c r="N12" s="4">
+        <v>1.8051536760197936E-2</v>
+      </c>
+      <c r="O12" s="4">
+        <v>3.6997136432840937E-4</v>
+      </c>
+      <c r="P12" s="4">
+        <v>-6.1308688662759264E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.28161278405128931</v>
+      </c>
+      <c r="C13" s="4">
         <v>-1.2017738306277972E-3</v>
       </c>
-      <c r="P3" s="4">
+      <c r="D13" s="4">
+        <v>5.6554129175789957E-3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>-1.292581853302221E-4</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1.8051536760197929E-2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>2.2470661711412227E-2</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-1.3296445028696763E-4</v>
+      </c>
+      <c r="I13" s="4">
+        <v>-7.7059339860927334E-2</v>
+      </c>
+      <c r="J13" s="4">
+        <v>4.1308486621334322E-4</v>
+      </c>
+      <c r="K13" s="4">
+        <v>-8.0466931609579628E-4</v>
+      </c>
+      <c r="L13" s="4">
+        <v>2.61109188486831E-5</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1.8051536760197936E-2</v>
+      </c>
+      <c r="N13" s="4">
+        <v>2.2470661711412238E-2</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2.7717215468628939E-4</v>
+      </c>
+      <c r="P13" s="4">
+        <v>-1.7778852112508695E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="5">
+        <v>-9.1094011810293862E-2</v>
+      </c>
+      <c r="C14" s="4">
         <v>-5.8053821501349986E-6</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="D14" s="4">
+        <v>9.9158329431915139E-5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>-2.2230649277966551E-6</v>
+      </c>
+      <c r="F14" s="4">
+        <v>3.6997136432840932E-4</v>
+      </c>
+      <c r="G14" s="4">
+        <v>2.7717215468628929E-4</v>
+      </c>
+      <c r="H14" s="4">
+        <v>2.3038586009592921E-5</v>
+      </c>
+      <c r="I14" s="4">
+        <v>-1.6822763833527488E-3</v>
+      </c>
+      <c r="J14" s="4">
+        <v>6.4916357692590757E-5</v>
+      </c>
+      <c r="K14" s="4">
+        <v>-1.375334198365108E-3</v>
+      </c>
+      <c r="L14" s="4">
+        <v>2.2307345343262723E-5</v>
+      </c>
+      <c r="M14" s="4">
+        <v>3.6997136432840937E-4</v>
+      </c>
+      <c r="N14" s="4">
+        <v>2.7717215468628939E-4</v>
+      </c>
+      <c r="O14" s="4">
+        <v>9.5494681945059552E-4</v>
+      </c>
+      <c r="P14" s="4">
+        <v>6.3497897579125051E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="5">
+        <v>-90.721983727043423</v>
+      </c>
+      <c r="C15" s="4">
         <v>-2.3068567761102582E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="5">
-        <v>2.5342748337312027</v>
-      </c>
-      <c r="D4" s="4">
-        <v>-1.0413845165261629E-2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.44461993036470349</v>
-      </c>
-      <c r="F4" s="4">
-        <v>-1.0648507729289675E-2</v>
-      </c>
-      <c r="G4" s="4">
-        <v>-1.6876698489636213E-3</v>
-      </c>
-      <c r="H4" s="4">
-        <v>5.6554129175876867E-3</v>
-      </c>
-      <c r="I4" s="4">
-        <v>3.1801245536059559E-4</v>
-      </c>
-      <c r="J4" s="4">
-        <v>-4.6134665027390236</v>
-      </c>
-      <c r="K4" s="4">
-        <v>9.9585808110615875E-4</v>
-      </c>
-      <c r="L4" s="4">
-        <v>-1.5547597491159387E-2</v>
-      </c>
-      <c r="M4" s="4">
-        <v>3.0601582871698542E-4</v>
-      </c>
-      <c r="N4" s="4">
-        <v>-1.6876698489273244E-3</v>
-      </c>
-      <c r="O4" s="4">
-        <v>5.6554129175789957E-3</v>
-      </c>
-      <c r="P4" s="4">
-        <v>9.9158329431915139E-5</v>
-      </c>
-      <c r="Q4" s="4">
+      <c r="D15" s="4">
         <v>0.19039686679488499</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5">
-        <v>-3.5462932151367588E-2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2.7761471073766179E-4</v>
-      </c>
-      <c r="E5" s="4">
-        <v>-1.0648507729289675E-2</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2.5624364995984031E-4</v>
-      </c>
-      <c r="G5" s="4">
-        <v>3.5708259359456035E-5</v>
-      </c>
-      <c r="H5" s="4">
-        <v>-1.2925818533043081E-4</v>
-      </c>
-      <c r="I5" s="4">
-        <v>-3.342489340852493E-6</v>
-      </c>
-      <c r="J5" s="4">
-        <v>0.1099138401010646</v>
-      </c>
-      <c r="K5" s="4">
-        <v>-2.6320624719421192E-5</v>
-      </c>
-      <c r="L5" s="4">
-        <v>3.8713232302430619E-4</v>
-      </c>
-      <c r="M5" s="4">
-        <v>-7.643592462939163E-6</v>
-      </c>
-      <c r="N5" s="4">
-        <v>3.5708259358577926E-5</v>
-      </c>
-      <c r="O5" s="4">
-        <v>-1.292581853302221E-4</v>
-      </c>
-      <c r="P5" s="4">
-        <v>-2.2230649277966551E-6</v>
-      </c>
-      <c r="Q5" s="4">
+      <c r="E15" s="4">
         <v>-4.7312092617540491E-3</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="5">
-        <v>3.963015435313573E-2</v>
-      </c>
-      <c r="D6" s="4">
-        <v>-2.6026573684412492E-4</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-1.6876698489636213E-3</v>
-      </c>
-      <c r="F6" s="4">
-        <v>3.5708259359456035E-5</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2.6695229473375381E-2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>1.8051536760197905E-2</v>
-      </c>
-      <c r="I6" s="4">
-        <v>-1.3805572918502144E-4</v>
-      </c>
-      <c r="J6" s="4">
-        <v>3.1667958915616943E-3</v>
-      </c>
-      <c r="K6" s="4">
-        <v>4.0361149902828821E-4</v>
-      </c>
-      <c r="L6" s="4">
-        <v>2.7228022868254521E-3</v>
-      </c>
-      <c r="M6" s="4">
-        <v>-4.6969842548320233E-5</v>
-      </c>
-      <c r="N6" s="4">
-        <v>2.6695229473375229E-2</v>
-      </c>
-      <c r="O6" s="4">
-        <v>1.8051536760197929E-2</v>
-      </c>
-      <c r="P6" s="4">
-        <v>3.6997136432840932E-4</v>
-      </c>
-      <c r="Q6" s="4">
+      <c r="F15" s="4">
         <v>-6.1308688662759236E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="5">
-        <v>0.2816127840512892</v>
-      </c>
-      <c r="D7" s="4">
-        <v>-1.2017738306277469E-3</v>
-      </c>
-      <c r="E7" s="4">
-        <v>5.6554129175876867E-3</v>
-      </c>
-      <c r="F7" s="4">
-        <v>-1.2925818533043081E-4</v>
-      </c>
-      <c r="G7" s="4">
-        <v>1.8051536760197905E-2</v>
-      </c>
-      <c r="H7" s="4">
-        <v>2.2470661711412248E-2</v>
-      </c>
-      <c r="I7" s="4">
-        <v>-1.3296445028694755E-4</v>
-      </c>
-      <c r="J7" s="4">
-        <v>-7.7059339860899495E-2</v>
-      </c>
-      <c r="K7" s="4">
-        <v>4.1308486621342085E-4</v>
-      </c>
-      <c r="L7" s="4">
-        <v>-8.0466931606505872E-4</v>
-      </c>
-      <c r="M7" s="4">
-        <v>2.6110918848061635E-5</v>
-      </c>
-      <c r="N7" s="4">
-        <v>1.8051536760197988E-2</v>
-      </c>
-      <c r="O7" s="4">
-        <v>2.2470661711412227E-2</v>
-      </c>
-      <c r="P7" s="4">
-        <v>2.7717215468628929E-4</v>
-      </c>
-      <c r="Q7" s="4">
+      <c r="G15" s="4">
         <v>-1.7778852112508667E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5">
-        <v>-3.7910917136234706E-3</v>
-      </c>
-      <c r="D8" s="4">
-        <v>1.7834668652452445E-4</v>
-      </c>
-      <c r="E8" s="4">
-        <v>3.1801245536059559E-4</v>
-      </c>
-      <c r="F8" s="4">
-        <v>-3.342489340852493E-6</v>
-      </c>
-      <c r="G8" s="4">
-        <v>-1.3805572918502144E-4</v>
-      </c>
-      <c r="H8" s="4">
-        <v>-1.3296445028694755E-4</v>
-      </c>
-      <c r="I8" s="4">
-        <v>6.0044282389084039E-4</v>
-      </c>
-      <c r="J8" s="4">
-        <v>-1.3794018318166575E-2</v>
-      </c>
-      <c r="K8" s="4">
-        <v>4.222582879213118E-6</v>
-      </c>
-      <c r="L8" s="4">
-        <v>8.5420470336085731E-5</v>
-      </c>
-      <c r="M8" s="4">
-        <v>-1.8808789396120872E-6</v>
-      </c>
-      <c r="N8" s="4">
-        <v>-1.380557291850026E-4</v>
-      </c>
-      <c r="O8" s="4">
-        <v>-1.3296445028696763E-4</v>
-      </c>
-      <c r="P8" s="4">
-        <v>2.3038586009592921E-5</v>
-      </c>
-      <c r="Q8" s="4">
+      <c r="H15" s="4">
         <v>-1.1738908394724051E-3</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5">
-        <v>-36.440248401675419</v>
-      </c>
-      <c r="D9" s="4">
-        <v>8.5711575329947665E-2</v>
-      </c>
-      <c r="E9" s="4">
-        <v>-4.6134665027390236</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.1099138401010646</v>
-      </c>
-      <c r="G9" s="4">
-        <v>3.1667958915616943E-3</v>
-      </c>
-      <c r="H9" s="4">
-        <v>-7.7059339860899495E-2</v>
-      </c>
-      <c r="I9" s="4">
-        <v>-1.3794018318166575E-2</v>
-      </c>
-      <c r="J9" s="4">
-        <v>48.290712115621027</v>
-      </c>
-      <c r="K9" s="4">
-        <v>-1.0116274927731983E-2</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0.1512957316426764</v>
-      </c>
-      <c r="M9" s="4">
-        <v>-2.972868257114937E-3</v>
-      </c>
-      <c r="N9" s="4">
-        <v>3.1667958914687253E-3</v>
-      </c>
-      <c r="O9" s="4">
-        <v>-7.7059339860927334E-2</v>
-      </c>
-      <c r="P9" s="4">
-        <v>-1.6822763833527488E-3</v>
-      </c>
-      <c r="Q9" s="4">
+      <c r="I15" s="4">
         <v>-1.83006133806348</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5">
-        <v>-0.72516532133752731</v>
-      </c>
-      <c r="D10" s="4">
-        <v>5.4643406357876264E-4</v>
-      </c>
-      <c r="E10" s="4">
-        <v>9.9585808110615875E-4</v>
-      </c>
-      <c r="F10" s="4">
-        <v>-2.6320624719421192E-5</v>
-      </c>
-      <c r="G10" s="4">
-        <v>4.0361149902828821E-4</v>
-      </c>
-      <c r="H10" s="4">
-        <v>4.1308486621342085E-4</v>
-      </c>
-      <c r="I10" s="4">
-        <v>4.222582879213118E-6</v>
-      </c>
-      <c r="J10" s="4">
-        <v>-1.0116274927731983E-2</v>
-      </c>
-      <c r="K10" s="4">
-        <v>2.0866752686068551E-2</v>
-      </c>
-      <c r="L10" s="4">
-        <v>6.1764252112221363E-3</v>
-      </c>
-      <c r="M10" s="4">
-        <v>-1.3628547951569179E-4</v>
-      </c>
-      <c r="N10" s="4">
-        <v>4.0361149902829667E-4</v>
-      </c>
-      <c r="O10" s="4">
-        <v>4.1308486621334322E-4</v>
-      </c>
-      <c r="P10" s="4">
-        <v>6.4916357692590757E-5</v>
-      </c>
-      <c r="Q10" s="4">
+      <c r="J15" s="4">
         <v>-8.0116635570056771E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5">
-        <v>6.905081187492188</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1.9305934574519595E-3</v>
-      </c>
-      <c r="E11" s="4">
-        <v>-1.5547597491159387E-2</v>
-      </c>
-      <c r="F11" s="4">
-        <v>3.8713232302430619E-4</v>
-      </c>
-      <c r="G11" s="4">
-        <v>2.7228022868254521E-3</v>
-      </c>
-      <c r="H11" s="4">
-        <v>-8.0466931606505872E-4</v>
-      </c>
-      <c r="I11" s="4">
-        <v>8.5420470336085731E-5</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0.1512957316426764</v>
-      </c>
-      <c r="K11" s="4">
-        <v>6.1764252112221363E-3</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0.98565093511474089</v>
-      </c>
-      <c r="M11" s="4">
-        <v>-2.0477000205447154E-2</v>
-      </c>
-      <c r="N11" s="4">
-        <v>2.7228022868038548E-3</v>
-      </c>
-      <c r="O11" s="4">
-        <v>-8.0466931609579628E-4</v>
-      </c>
-      <c r="P11" s="4">
-        <v>-1.375334198365108E-3</v>
-      </c>
-      <c r="Q11" s="4">
+      <c r="K15" s="4">
         <v>-11.789704530453577</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="5">
-        <v>-0.12868226744750794</v>
-      </c>
-      <c r="D12" s="4">
-        <v>-3.9215826092171553E-5</v>
-      </c>
-      <c r="E12" s="4">
-        <v>3.0601582871698542E-4</v>
-      </c>
-      <c r="F12" s="4">
-        <v>-7.643592462939163E-6</v>
-      </c>
-      <c r="G12" s="4">
-        <v>-4.6969842548320233E-5</v>
-      </c>
-      <c r="H12" s="4">
-        <v>2.6110918848061635E-5</v>
-      </c>
-      <c r="I12" s="4">
-        <v>-1.8808789396120872E-6</v>
-      </c>
-      <c r="J12" s="4">
-        <v>-2.972868257114937E-3</v>
-      </c>
-      <c r="K12" s="4">
-        <v>-1.3628547951569179E-4</v>
-      </c>
-      <c r="L12" s="4">
-        <v>-2.0477000205447154E-2</v>
-      </c>
-      <c r="M12" s="4">
-        <v>4.2629215885812023E-4</v>
-      </c>
-      <c r="N12" s="4">
-        <v>-4.6969842548117216E-5</v>
-      </c>
-      <c r="O12" s="4">
-        <v>2.61109188486831E-5</v>
-      </c>
-      <c r="P12" s="4">
-        <v>2.2307345343262723E-5</v>
-      </c>
-      <c r="Q12" s="4">
+      <c r="L15" s="4">
         <v>0.2445039237348734</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="5">
-        <v>3.9630154353135744E-2</v>
-      </c>
-      <c r="D13" s="4">
-        <v>-2.602657368440803E-4</v>
-      </c>
-      <c r="E13" s="4">
-        <v>-1.6876698489273244E-3</v>
-      </c>
-      <c r="F13" s="4">
-        <v>3.5708259358577926E-5</v>
-      </c>
-      <c r="G13" s="4">
-        <v>2.6695229473375229E-2</v>
-      </c>
-      <c r="H13" s="4">
-        <v>1.8051536760197988E-2</v>
-      </c>
-      <c r="I13" s="4">
-        <v>-1.380557291850026E-4</v>
-      </c>
-      <c r="J13" s="4">
-        <v>3.1667958914687253E-3</v>
-      </c>
-      <c r="K13" s="4">
-        <v>4.0361149902829667E-4</v>
-      </c>
-      <c r="L13" s="4">
-        <v>2.7228022868038548E-3</v>
-      </c>
-      <c r="M13" s="4">
-        <v>-4.6969842548117216E-5</v>
-      </c>
-      <c r="N13" s="4">
-        <v>2.6695229473375232E-2</v>
-      </c>
-      <c r="O13" s="4">
-        <v>1.8051536760197936E-2</v>
-      </c>
-      <c r="P13" s="4">
-        <v>3.6997136432840937E-4</v>
-      </c>
-      <c r="Q13" s="4">
+      <c r="M15" s="4">
         <v>-6.1308688662759264E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="5">
-        <v>0.28161278405128931</v>
-      </c>
-      <c r="D14" s="4">
-        <v>-1.2017738306277972E-3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>5.6554129175789957E-3</v>
-      </c>
-      <c r="F14" s="4">
-        <v>-1.292581853302221E-4</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1.8051536760197929E-2</v>
-      </c>
-      <c r="H14" s="4">
-        <v>2.2470661711412227E-2</v>
-      </c>
-      <c r="I14" s="4">
-        <v>-1.3296445028696763E-4</v>
-      </c>
-      <c r="J14" s="4">
-        <v>-7.7059339860927334E-2</v>
-      </c>
-      <c r="K14" s="4">
-        <v>4.1308486621334322E-4</v>
-      </c>
-      <c r="L14" s="4">
-        <v>-8.0466931609579628E-4</v>
-      </c>
-      <c r="M14" s="4">
-        <v>2.61109188486831E-5</v>
-      </c>
-      <c r="N14" s="4">
-        <v>1.8051536760197936E-2</v>
-      </c>
-      <c r="O14" s="4">
-        <v>2.2470661711412238E-2</v>
-      </c>
-      <c r="P14" s="4">
-        <v>2.7717215468628939E-4</v>
-      </c>
-      <c r="Q14" s="4">
+      <c r="N15" s="4">
         <v>-1.7778852112508695E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="5">
-        <v>-9.1094011810293862E-2</v>
-      </c>
-      <c r="D15" s="4">
-        <v>-5.8053821501349986E-6</v>
-      </c>
-      <c r="E15" s="4">
-        <v>9.9158329431915139E-5</v>
-      </c>
-      <c r="F15" s="4">
-        <v>-2.2230649277966551E-6</v>
-      </c>
-      <c r="G15" s="4">
-        <v>3.6997136432840932E-4</v>
-      </c>
-      <c r="H15" s="4">
-        <v>2.7717215468628929E-4</v>
-      </c>
-      <c r="I15" s="4">
-        <v>2.3038586009592921E-5</v>
-      </c>
-      <c r="J15" s="4">
-        <v>-1.6822763833527488E-3</v>
-      </c>
-      <c r="K15" s="4">
-        <v>6.4916357692590757E-5</v>
-      </c>
-      <c r="L15" s="4">
-        <v>-1.375334198365108E-3</v>
-      </c>
-      <c r="M15" s="4">
-        <v>2.2307345343262723E-5</v>
-      </c>
-      <c r="N15" s="4">
-        <v>3.6997136432840937E-4</v>
-      </c>
       <c r="O15" s="4">
-        <v>2.7717215468628939E-4</v>
+        <v>6.3497897579125051E-3</v>
       </c>
       <c r="P15" s="4">
-        <v>9.5494681945059552E-4</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>6.3497897579125051E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5">
-        <v>-90.721983727043423</v>
-      </c>
-      <c r="D16" s="4">
-        <v>-2.3068567761102582E-2</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.19039686679488499</v>
-      </c>
-      <c r="F16" s="4">
-        <v>-4.7312092617540491E-3</v>
-      </c>
-      <c r="G16" s="4">
-        <v>-6.1308688662759236E-2</v>
-      </c>
-      <c r="H16" s="4">
-        <v>-1.7778852112508667E-2</v>
-      </c>
-      <c r="I16" s="4">
-        <v>-1.1738908394724051E-3</v>
-      </c>
-      <c r="J16" s="4">
-        <v>-1.83006133806348</v>
-      </c>
-      <c r="K16" s="4">
-        <v>-8.0116635570056771E-2</v>
-      </c>
-      <c r="L16" s="4">
-        <v>-11.789704530453577</v>
-      </c>
-      <c r="M16" s="4">
-        <v>0.2445039237348734</v>
-      </c>
-      <c r="N16" s="4">
-        <v>-6.1308688662759264E-2</v>
-      </c>
-      <c r="O16" s="4">
-        <v>-1.7778852112508695E-2</v>
-      </c>
-      <c r="P16" s="4">
-        <v>6.3497897579125051E-3</v>
-      </c>
-      <c r="Q16" s="4">
         <v>141.44420667362533</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Small updates to Excel files
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{768C2E1A-BF06-4059-81BD-146F48A1ABF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A757B2C-8655-4AE8-B476-32F1199B2823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="HU_E1a" sheetId="45" r:id="rId2"/>
     <sheet name="HU_E1b" sheetId="46" r:id="rId3"/>
     <sheet name="HU_E2a" sheetId="47" r:id="rId4"/>
+    <sheet name="HU_E2a (2)" sheetId="48" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -120,9 +121,6 @@
   </si>
   <si>
     <t>HUA</t>
-  </si>
-  <si>
-    <t>REGREESOR</t>
   </si>
   <si>
     <t>Deh_c3_High_L1</t>
@@ -654,7 +652,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -920,7 +918,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
@@ -1081,7 +1079,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" s="5">
         <v>0.20548480534059291</v>
@@ -1482,15 +1480,263 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4166C8A3-8125-479C-A99A-1257D5F59E53}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="26.5703125" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.41379566713805094</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1.8006708482058549E-2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>-1.0413845165261629E-2</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2.7761471073766179E-4</v>
+      </c>
+      <c r="F2" s="4">
+        <v>-2.6026573684412492E-4</v>
+      </c>
+      <c r="G2" s="4">
+        <v>-1.2017738306277469E-3</v>
+      </c>
+      <c r="H2" s="4">
+        <v>1.7834668652452445E-4</v>
+      </c>
+      <c r="I2" s="4">
+        <v>8.5711575329947665E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2.5342748337312027</v>
+      </c>
+      <c r="C3" s="4">
+        <v>-1.0413845165261629E-2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0.44461993036470349</v>
+      </c>
+      <c r="E3" s="4">
+        <v>-1.0648507729289675E-2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-1.6876698489636213E-3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5.6554129175876867E-3</v>
+      </c>
+      <c r="H3" s="4">
+        <v>3.1801245536059559E-4</v>
+      </c>
+      <c r="I3" s="4">
+        <v>-4.6134665027390236</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="5">
+        <v>-3.5462932151367588E-2</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.7761471073766179E-4</v>
+      </c>
+      <c r="D4" s="4">
+        <v>-1.0648507729289675E-2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>2.5624364995984031E-4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3.5708259359456035E-5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>-1.2925818533043081E-4</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-3.342489340852493E-6</v>
+      </c>
+      <c r="I4" s="4">
+        <v>0.1099138401010646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="5">
+        <v>3.963015435313573E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>-2.6026573684412492E-4</v>
+      </c>
+      <c r="D5" s="4">
+        <v>-1.6876698489636213E-3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>3.5708259359456035E-5</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2.6695229473375381E-2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.8051536760197905E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-1.3805572918502144E-4</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3.1667958915616943E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.2816127840512892</v>
+      </c>
+      <c r="C6" s="4">
+        <v>-1.2017738306277469E-3</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5.6554129175876867E-3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>-1.2925818533043081E-4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1.8051536760197905E-2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>2.2470661711412248E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-1.3296445028694755E-4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>-7.7059339860899495E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="5">
+        <v>-3.7910917136234706E-3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1.7834668652452445E-4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3.1801245536059559E-4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>-3.342489340852493E-6</v>
+      </c>
+      <c r="F7" s="4">
+        <v>-1.3805572918502144E-4</v>
+      </c>
+      <c r="G7" s="4">
+        <v>-1.3296445028694755E-4</v>
+      </c>
+      <c r="H7" s="4">
+        <v>6.0044282389084039E-4</v>
+      </c>
+      <c r="I7" s="4">
+        <v>-1.3794018318166575E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="5">
+        <v>-36.440248401675419</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8.5711575329947665E-2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>-4.6134665027390236</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.1099138401010646</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3.1667958915616943E-3</v>
+      </c>
+      <c r="G8" s="4">
+        <v>-7.7059339860899495E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-1.3794018318166575E-2</v>
+      </c>
+      <c r="I8" s="4">
+        <v>48.290712115621027</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4668BA-9B37-4004-9304-470683CE908D}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" style="4" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
@@ -1501,51 +1747,51 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5">
         <v>0.41379566713805094</v>
@@ -1595,7 +1841,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="5">
         <v>2.5342748337312027</v>
@@ -1645,7 +1891,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="5">
         <v>-3.5462932151367588E-2</v>
@@ -1695,7 +1941,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5">
         <v>3.963015435313573E-2</v>
@@ -1745,7 +1991,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="5">
         <v>0.2816127840512892</v>
@@ -1795,7 +2041,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5">
         <v>-3.7910917136234706E-3</v>
@@ -1845,7 +2091,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="5">
         <v>-36.440248401675419</v>
@@ -1895,7 +2141,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="5">
         <v>-0.72516532133752731</v>
@@ -1945,7 +2191,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="5">
         <v>6.905081187492188</v>
@@ -1995,7 +2241,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="5">
         <v>-0.12868226744750794</v>
@@ -2045,7 +2291,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" s="5">
         <v>3.9630154353135744E-2</v>
@@ -2095,7 +2341,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
         <v>0.28161278405128931</v>
@@ -2145,7 +2391,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="5">
         <v>-9.1094011810293862E-2</v>
@@ -2195,7 +2441,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="5">
         <v>-90.721983727043423</v>

</xml_diff>

<commit_message>
Complete update of the estimates
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A757B2C-8655-4AE8-B476-32F1199B2823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEE869B-1818-4C80-8E18-C06F6AE02DEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
@@ -16,8 +16,7 @@
     <sheet name="Info" sheetId="12" r:id="rId1"/>
     <sheet name="HU_E1a" sheetId="45" r:id="rId2"/>
     <sheet name="HU_E1b" sheetId="46" r:id="rId3"/>
-    <sheet name="HU_E2a" sheetId="47" r:id="rId4"/>
-    <sheet name="HU_E2a (2)" sheetId="48" r:id="rId5"/>
+    <sheet name="HU_E2a" sheetId="48" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="43">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -1479,259 +1478,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4166C8A3-8125-479C-A99A-1257D5F59E53}">
-  <dimension ref="A1:I8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.5703125" style="4" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="5">
-        <v>0.41379566713805094</v>
-      </c>
-      <c r="C2" s="4">
-        <v>1.8006708482058549E-2</v>
-      </c>
-      <c r="D2" s="4">
-        <v>-1.0413845165261629E-2</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2.7761471073766179E-4</v>
-      </c>
-      <c r="F2" s="4">
-        <v>-2.6026573684412492E-4</v>
-      </c>
-      <c r="G2" s="4">
-        <v>-1.2017738306277469E-3</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1.7834668652452445E-4</v>
-      </c>
-      <c r="I2" s="4">
-        <v>8.5711575329947665E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="5">
-        <v>2.5342748337312027</v>
-      </c>
-      <c r="C3" s="4">
-        <v>-1.0413845165261629E-2</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.44461993036470349</v>
-      </c>
-      <c r="E3" s="4">
-        <v>-1.0648507729289675E-2</v>
-      </c>
-      <c r="F3" s="4">
-        <v>-1.6876698489636213E-3</v>
-      </c>
-      <c r="G3" s="4">
-        <v>5.6554129175876867E-3</v>
-      </c>
-      <c r="H3" s="4">
-        <v>3.1801245536059559E-4</v>
-      </c>
-      <c r="I3" s="4">
-        <v>-4.6134665027390236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="5">
-        <v>-3.5462932151367588E-2</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2.7761471073766179E-4</v>
-      </c>
-      <c r="D4" s="4">
-        <v>-1.0648507729289675E-2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2.5624364995984031E-4</v>
-      </c>
-      <c r="F4" s="4">
-        <v>3.5708259359456035E-5</v>
-      </c>
-      <c r="G4" s="4">
-        <v>-1.2925818533043081E-4</v>
-      </c>
-      <c r="H4" s="4">
-        <v>-3.342489340852493E-6</v>
-      </c>
-      <c r="I4" s="4">
-        <v>0.1099138401010646</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="5">
-        <v>3.963015435313573E-2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>-2.6026573684412492E-4</v>
-      </c>
-      <c r="D5" s="4">
-        <v>-1.6876698489636213E-3</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.5708259359456035E-5</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2.6695229473375381E-2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>1.8051536760197905E-2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>-1.3805572918502144E-4</v>
-      </c>
-      <c r="I5" s="4">
-        <v>3.1667958915616943E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0.2816127840512892</v>
-      </c>
-      <c r="C6" s="4">
-        <v>-1.2017738306277469E-3</v>
-      </c>
-      <c r="D6" s="4">
-        <v>5.6554129175876867E-3</v>
-      </c>
-      <c r="E6" s="4">
-        <v>-1.2925818533043081E-4</v>
-      </c>
-      <c r="F6" s="4">
-        <v>1.8051536760197905E-2</v>
-      </c>
-      <c r="G6" s="4">
-        <v>2.2470661711412248E-2</v>
-      </c>
-      <c r="H6" s="4">
-        <v>-1.3296445028694755E-4</v>
-      </c>
-      <c r="I6" s="4">
-        <v>-7.7059339860899495E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="5">
-        <v>-3.7910917136234706E-3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1.7834668652452445E-4</v>
-      </c>
-      <c r="D7" s="4">
-        <v>3.1801245536059559E-4</v>
-      </c>
-      <c r="E7" s="4">
-        <v>-3.342489340852493E-6</v>
-      </c>
-      <c r="F7" s="4">
-        <v>-1.3805572918502144E-4</v>
-      </c>
-      <c r="G7" s="4">
-        <v>-1.3296445028694755E-4</v>
-      </c>
-      <c r="H7" s="4">
-        <v>6.0044282389084039E-4</v>
-      </c>
-      <c r="I7" s="4">
-        <v>-1.3794018318166575E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="5">
-        <v>-36.440248401675419</v>
-      </c>
-      <c r="C8" s="4">
-        <v>8.5711575329947665E-2</v>
-      </c>
-      <c r="D8" s="4">
-        <v>-4.6134665027390236</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.1099138401010646</v>
-      </c>
-      <c r="F8" s="4">
-        <v>3.1667958915616943E-3</v>
-      </c>
-      <c r="G8" s="4">
-        <v>-7.7059339860899495E-2</v>
-      </c>
-      <c r="H8" s="4">
-        <v>-1.3794018318166575E-2</v>
-      </c>
-      <c r="I8" s="4">
-        <v>48.290712115621027</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C4668BA-9B37-4004-9304-470683CE908D}">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Update education and health estimates
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4D2401-03E2-4DD5-89E2-188BFED96C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2344EB1-6822-4C87-BFEB-1B3192FFEFDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="919" activeTab="3" xr2:uid="{536B1BCD-7004-4A8B-8363-6CEFA8439CE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="12" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="41">
   <si>
     <t>REGRESSOR</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>HUB_</t>
+  </si>
+  <si>
+    <t>Dag_sq_</t>
   </si>
 </sst>
 </file>
@@ -1499,7 +1502,7 @@
         <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
         <v>31</v>
@@ -1701,7 +1704,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>-3.5462932151367588E-2</v>

</xml_diff>

<commit_message>
Education process E2a update
</commit_message>
<xml_diff>
--- a/input/reg_education.xlsx
+++ b/input/reg_education.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPaths_HU\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7573AA33-CBB6-485C-AF00-CCF6B37039B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D42C66D-EBDE-4B2F-BBDF-0D8BCF8219F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="46">
   <si>
     <t>Description:</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Dag_sq_Low</t>
   </si>
   <si>
-    <t>Y2020_Low</t>
-  </si>
-  <si>
     <t>Y2021_Low</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Dag_sq_Medium</t>
   </si>
   <si>
-    <t>Y2020_Medium</t>
-  </si>
-  <si>
     <t>Y2021_Medium</t>
   </si>
   <si>
@@ -164,13 +158,16 @@
   </si>
   <si>
     <t>PL6_</t>
+  </si>
+  <si>
+    <t>Y2020_</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="77" x14ac:knownFonts="1">
+  <fonts count="57" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -188,106 +185,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -566,273 +463,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="100">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1271,7 +902,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1328,46 +959,7 @@
     <xf numFmtId="2" fontId="54" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="55" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="56" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="57" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="58" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="59" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="60" fillId="0" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="61" fillId="0" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="62" fillId="0" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="63" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="64" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="65" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="66" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="67" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="68" fillId="0" borderId="82" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="69" fillId="0" borderId="84" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="70" fillId="0" borderId="86" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="71" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="72" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="73" fillId="0" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="74" fillId="0" borderId="94" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="75" fillId="0" borderId="96" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="76" fillId="0" borderId="98" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="83" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="85" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="91" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="95" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="97" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="99" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1756,11 +1348,11 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="56" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1793,16 +1385,16 @@
         <v>14</v>
       </c>
       <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" t="s">
-        <v>40</v>
       </c>
       <c r="J1" t="s">
         <v>15</v>
@@ -1941,8 +1533,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="96" t="s">
-        <v>37</v>
+      <c r="A5" s="57" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="11">
         <v>6.4190072143362293E-3</v>
@@ -1982,8 +1574,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
-        <v>38</v>
+      <c r="A6" s="58" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="12">
         <v>-2.7386561938964729E-2</v>
@@ -2023,8 +1615,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="98" t="s">
-        <v>39</v>
+      <c r="A7" s="59" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="13">
         <v>1.8886269847779816E-2</v>
@@ -2064,8 +1656,8 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
-        <v>40</v>
+      <c r="A8" s="60" t="s">
+        <v>38</v>
       </c>
       <c r="B8" s="14">
         <v>0.10230029249748195</v>
@@ -2318,16 +1910,16 @@
         <v>23</v>
       </c>
       <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
-      </c>
-      <c r="M1" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" t="s">
-        <v>40</v>
       </c>
       <c r="O1" t="s">
         <v>15</v>
@@ -2791,8 +2383,8 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="100" t="s">
-        <v>37</v>
+      <c r="A10" s="61" t="s">
+        <v>35</v>
       </c>
       <c r="B10" s="41">
         <v>-0.11280370100427836</v>
@@ -2848,7 +2440,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="42" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="43">
         <v>0.14765801784257579</v>
@@ -2904,7 +2496,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="44" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B12" s="45">
         <v>3.7086456144431824E-2</v>
@@ -2960,7 +2552,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="47">
         <v>0.14286262179509499</v>
@@ -3245,7 +2837,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:T19"/>
+  <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3254,73 +2846,70 @@
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="94" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" t="s">
+        <v>40</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="94" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="94" t="s">
-        <v>25</v>
-      </c>
-      <c r="H1" s="94" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" s="94" t="s">
-        <v>27</v>
-      </c>
-      <c r="J1" s="94" t="s">
+      <c r="R1" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="94" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="94" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="94" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="94" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="94" t="s">
-        <v>32</v>
-      </c>
-      <c r="P1" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q1" s="94" t="s">
-        <v>43</v>
-      </c>
-      <c r="R1" s="94" t="s">
-        <v>34</v>
-      </c>
-      <c r="S1" s="94" t="s">
-        <v>35</v>
-      </c>
-      <c r="T1" s="94" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="62">
+      <c r="B2">
         <v>-0.42810985445751515</v>
       </c>
       <c r="C2">
@@ -3336,19 +2925,19 @@
         <v>-2.2180042805181494E-4</v>
       </c>
       <c r="G2">
+        <v>-5.5324896085389092E-4</v>
+      </c>
+      <c r="H2">
         <v>-1.180705777733338E-3</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>-1.5585750691915812E-2</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3.6250936971131149E-4</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1.3294217299166361E-2</v>
-      </c>
-      <c r="K2">
-        <v>-5.5324896085389092E-4</v>
       </c>
       <c r="L2">
         <v>1.7198721939736899E-3</v>
@@ -3369,20 +2958,17 @@
         <v>1.0783269614622034E-2</v>
       </c>
       <c r="R2">
-        <v>-5.5324896085405637E-4</v>
+        <v>2.2233406111747426E-3</v>
       </c>
       <c r="S2">
-        <v>2.2233406111747426E-3</v>
-      </c>
-      <c r="T2">
         <v>0.13936901697517656</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="77" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="63">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
         <v>-0.34117979954907873</v>
       </c>
       <c r="C3">
@@ -3398,19 +2984,19 @@
         <v>2.5484272463857942E-5</v>
       </c>
       <c r="G3">
+        <v>8.7304371488515758E-4</v>
+      </c>
+      <c r="H3">
         <v>-9.7733728947234193E-4</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>-5.7399666079350764E-3</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1.3896885381833694E-4</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>1.3082891144080707E-2</v>
-      </c>
-      <c r="K3">
-        <v>8.7304371488515758E-4</v>
       </c>
       <c r="L3">
         <v>-1.6250052708554575E-3</v>
@@ -3431,20 +3017,17 @@
         <v>1.1677869825386843E-2</v>
       </c>
       <c r="R3">
-        <v>8.7304371488505599E-4</v>
+        <v>-7.5774829137869679E-3</v>
       </c>
       <c r="S3">
-        <v>-7.5774829137869679E-3</v>
-      </c>
-      <c r="T3">
         <v>0.22634927920258352</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="64">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4">
         <v>-3.6348095675537533E-2</v>
       </c>
       <c r="C4">
@@ -3460,19 +3043,19 @@
         <v>5.5394637342001934E-5</v>
       </c>
       <c r="G4">
+        <v>4.6451815529680723E-4</v>
+      </c>
+      <c r="H4">
         <v>-1.1405287225127536E-3</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>-1.0364286813646512E-2</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2.4404140208148135E-4</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1.2741260351183524E-2</v>
-      </c>
-      <c r="K4">
-        <v>4.6451815529680723E-4</v>
       </c>
       <c r="L4">
         <v>1.7176935826364362E-3</v>
@@ -3493,20 +3076,17 @@
         <v>1.1819067310418135E-2</v>
       </c>
       <c r="R4">
-        <v>4.6451815529675086E-4</v>
+        <v>-1.0734460577005167E-3</v>
       </c>
       <c r="S4">
-        <v>-1.0734460577005167E-3</v>
-      </c>
-      <c r="T4">
         <v>0.27644900393323169</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="65">
+      <c r="B5">
         <v>-3.7739823369109457E-2</v>
       </c>
       <c r="C5">
@@ -3522,19 +3102,19 @@
         <v>2.4999335300961021E-4</v>
       </c>
       <c r="G5">
+        <v>-9.5629351866941101E-4</v>
+      </c>
+      <c r="H5">
         <v>-5.3651733503946647E-5</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>3.0849436426212684E-4</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>-4.7871242250204817E-6</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>-5.5210167459380708E-5</v>
-      </c>
-      <c r="K5">
-        <v>-9.5629351866941101E-4</v>
       </c>
       <c r="L5">
         <v>-1.2180629628201398E-3</v>
@@ -3555,330 +3135,312 @@
         <v>-4.192765687167704E-5</v>
       </c>
       <c r="R5">
-        <v>-9.5629351866939605E-4</v>
+        <v>-2.9275421706408105E-3</v>
       </c>
       <c r="S5">
-        <v>-2.9275421706408105E-3</v>
-      </c>
-      <c r="T5">
         <v>2.1657007298017561E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="80" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6">
+        <v>-1.2073265405911591</v>
+      </c>
+      <c r="C6">
+        <v>-5.5324896085389092E-4</v>
+      </c>
+      <c r="D6">
+        <v>8.7304371488515758E-4</v>
+      </c>
+      <c r="E6">
+        <v>4.6451815529680723E-4</v>
+      </c>
+      <c r="F6">
+        <v>-9.5629351866941101E-4</v>
+      </c>
+      <c r="G6">
+        <v>6.0474412373201426E-2</v>
+      </c>
+      <c r="H6">
+        <v>-2.9223241728487236E-3</v>
+      </c>
+      <c r="I6">
+        <v>5.7739783668752098E-3</v>
+      </c>
+      <c r="J6">
+        <v>-8.3991358960767634E-5</v>
+      </c>
+      <c r="K6">
+        <v>3.0891323863099294E-3</v>
+      </c>
+      <c r="L6">
+        <v>1.2048822111075103E-2</v>
+      </c>
+      <c r="M6">
+        <v>-6.8483072996334715E-2</v>
+      </c>
+      <c r="N6">
+        <v>3.1804823520365563E-4</v>
+      </c>
+      <c r="O6">
+        <v>6.6612731888889276E-3</v>
+      </c>
+      <c r="P6">
+        <v>-1.1980635301275539E-4</v>
+      </c>
+      <c r="Q6">
+        <v>1.4408950208657876E-3</v>
+      </c>
+      <c r="R6">
+        <v>1.3892230893192671E-2</v>
+      </c>
+      <c r="S6">
+        <v>-7.6393196346831616E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="58">
+      <c r="B7">
         <v>-0.11581821838596346</v>
       </c>
-      <c r="C6">
+      <c r="C7">
         <v>-1.180705777733338E-3</v>
       </c>
-      <c r="D6">
+      <c r="D7">
         <v>-9.7733728947234193E-4</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>-1.1405287225127536E-3</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>-5.3651733503946647E-5</v>
       </c>
-      <c r="G6">
+      <c r="G7">
+        <v>-2.9223241728487236E-3</v>
+      </c>
+      <c r="H7">
         <v>1.3635343971217977E-2</v>
       </c>
-      <c r="H6">
+      <c r="I7">
         <v>6.735557964405274E-3</v>
       </c>
-      <c r="I6">
+      <c r="J7">
         <v>-1.7622103882496294E-4</v>
       </c>
-      <c r="J6">
+      <c r="K7">
         <v>-3.7274412302870348E-4</v>
       </c>
-      <c r="K6">
-        <v>-2.9223241728487236E-3</v>
-      </c>
-      <c r="L6">
+      <c r="L7">
         <v>8.3432692270468851E-4</v>
       </c>
-      <c r="M6">
+      <c r="M7">
         <v>-6.9385984347325624E-2</v>
       </c>
-      <c r="N6">
+      <c r="N7">
         <v>2.0875792007095254E-3</v>
       </c>
-      <c r="O6">
+      <c r="O7">
         <v>7.6436418682022111E-3</v>
       </c>
-      <c r="P6">
+      <c r="P7">
         <v>-1.7606722060131089E-4</v>
       </c>
-      <c r="Q6">
+      <c r="Q7">
         <v>-5.0749219320046779E-4</v>
       </c>
-      <c r="R6">
-        <v>-2.9223241728486274E-3</v>
-      </c>
-      <c r="S6">
+      <c r="R7">
         <v>-3.0264532465248267E-3</v>
       </c>
-      <c r="T6">
+      <c r="S7">
         <v>-8.1502980435032235E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="59">
+      <c r="B8">
         <v>2.5635616884438681</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>-1.5585750691915812E-2</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>-5.7399666079350764E-3</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>-1.0364286813646512E-2</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>3.0849436426212684E-4</v>
       </c>
-      <c r="G7">
+      <c r="G8">
+        <v>5.7739783668752098E-3</v>
+      </c>
+      <c r="H8">
         <v>6.735557964405274E-3</v>
       </c>
-      <c r="H7">
+      <c r="I8">
         <v>0.21882397591414104</v>
       </c>
-      <c r="I7">
+      <c r="J8">
         <v>-5.1797680717706601E-3</v>
       </c>
-      <c r="J7">
+      <c r="K8">
         <v>-7.9806840764326537E-3</v>
       </c>
-      <c r="K7">
-        <v>5.7739783668752098E-3</v>
-      </c>
-      <c r="L7">
+      <c r="L8">
         <v>2.1888593728654135E-2</v>
       </c>
-      <c r="M7">
+      <c r="M8">
         <v>-2.2853612385423787</v>
       </c>
-      <c r="N7">
+      <c r="N8">
         <v>2.5542802199271519E-4</v>
       </c>
-      <c r="O7">
+      <c r="O8">
         <v>0.34900827040695148</v>
       </c>
-      <c r="P7">
+      <c r="P8">
         <v>-7.7847833132934641E-3</v>
       </c>
-      <c r="Q7">
+      <c r="Q8">
         <v>2.4333200146942624E-3</v>
       </c>
-      <c r="R7">
-        <v>5.7739783668786515E-3</v>
-      </c>
-      <c r="S7">
+      <c r="R8">
         <v>0.11744784111344853</v>
       </c>
-      <c r="T7">
+      <c r="S8">
         <v>-3.8831443961643544</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="82" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="60">
+      <c r="B9">
         <v>-4.8066717422685763E-2</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>3.6250936971131149E-4</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>1.3896885381833694E-4</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>2.4404140208148135E-4</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>-4.7871242250204817E-6</v>
       </c>
-      <c r="G8">
+      <c r="G9">
+        <v>-8.3991358960767634E-5</v>
+      </c>
+      <c r="H9">
         <v>-1.7622103882496294E-4</v>
       </c>
-      <c r="H8">
+      <c r="I9">
         <v>-5.1797680717706601E-3</v>
       </c>
-      <c r="I8">
+      <c r="J9">
         <v>1.234500603005432E-4</v>
       </c>
-      <c r="J8">
+      <c r="K9">
         <v>1.8965539691813502E-4</v>
       </c>
-      <c r="K8">
-        <v>-8.3991358960767634E-5</v>
-      </c>
-      <c r="L8">
+      <c r="L9">
         <v>-4.8190179695063891E-4</v>
       </c>
-      <c r="M8">
+      <c r="M9">
         <v>5.3741914882832531E-2</v>
       </c>
-      <c r="N8">
+      <c r="N9">
         <v>-1.0167460514225873E-5</v>
       </c>
-      <c r="O8">
+      <c r="O9">
         <v>-8.7009815503651111E-3</v>
       </c>
-      <c r="P8">
+      <c r="P9">
         <v>1.9419292552027689E-4</v>
       </c>
-      <c r="Q8">
+      <c r="Q9">
         <v>-6.8682784559759638E-5</v>
       </c>
-      <c r="R8">
-        <v>-8.3991358960842227E-5</v>
-      </c>
-      <c r="S8">
+      <c r="R9">
         <v>-2.9384538952128628E-3</v>
       </c>
-      <c r="T8">
+      <c r="S9">
         <v>9.6725413434437524E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="83" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" s="61">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10">
         <v>-0.36034842905588782</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>1.3294217299166361E-2</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>1.3082891144080707E-2</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>1.2741260351183524E-2</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>-5.5210167459380708E-5</v>
       </c>
-      <c r="G9">
+      <c r="G10">
+        <v>3.0891323863099294E-3</v>
+      </c>
+      <c r="H10">
         <v>-3.7274412302870348E-4</v>
       </c>
-      <c r="H9">
+      <c r="I10">
         <v>-7.9806840764326537E-3</v>
       </c>
-      <c r="I9">
+      <c r="J10">
         <v>1.8965539691813502E-4</v>
       </c>
-      <c r="J9">
+      <c r="K10">
         <v>3.2393903845846644E-2</v>
       </c>
-      <c r="K9">
-        <v>3.0891323863099294E-3</v>
-      </c>
-      <c r="L9">
+      <c r="L10">
         <v>-8.1010104598913039E-6</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>6.9902796488167718E-2</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>-1.0890264547783091E-3</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>-1.4468652241800294E-2</v>
       </c>
-      <c r="P9">
+      <c r="P10">
         <v>3.1697426898209086E-4</v>
       </c>
-      <c r="Q9">
+      <c r="Q10">
         <v>1.2012384574993356E-2</v>
       </c>
-      <c r="R9">
-        <v>3.0891323863097963E-3</v>
-      </c>
-      <c r="S9">
+      <c r="R10">
         <v>1.3457265497723823E-3</v>
       </c>
-      <c r="T9">
+      <c r="S10">
         <v>0.15531469348685284</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="84" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="66">
-        <v>-1.2073265405911591</v>
-      </c>
-      <c r="C10">
-        <v>-5.5324896085389092E-4</v>
-      </c>
-      <c r="D10">
-        <v>8.7304371488515758E-4</v>
-      </c>
-      <c r="E10">
-        <v>4.6451815529680723E-4</v>
-      </c>
-      <c r="F10">
-        <v>-9.5629351866941101E-4</v>
-      </c>
-      <c r="G10">
-        <v>-2.9223241728487236E-3</v>
-      </c>
-      <c r="H10">
-        <v>5.7739783668752098E-3</v>
-      </c>
-      <c r="I10">
-        <v>-8.3991358960767634E-5</v>
-      </c>
-      <c r="J10">
-        <v>3.0891323863099294E-3</v>
-      </c>
-      <c r="K10">
-        <v>6.0474412373201426E-2</v>
-      </c>
-      <c r="L10">
-        <v>1.2048822111075103E-2</v>
-      </c>
-      <c r="M10">
-        <v>-6.8483072996334715E-2</v>
-      </c>
-      <c r="N10">
-        <v>3.1804823520365563E-4</v>
-      </c>
-      <c r="O10">
-        <v>6.6612731888889276E-3</v>
-      </c>
-      <c r="P10">
-        <v>-1.1980635301275539E-4</v>
-      </c>
-      <c r="Q10">
-        <v>1.4408950208657876E-3</v>
-      </c>
-      <c r="R10">
-        <v>6.0474412373201447E-2</v>
-      </c>
-      <c r="S10">
-        <v>1.3892230893192671E-2</v>
-      </c>
-      <c r="T10">
-        <v>-7.6393196346831616E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="85" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="67">
+      <c r="B11">
         <v>0.38267691211503663</v>
       </c>
       <c r="C11">
@@ -3894,19 +3456,19 @@
         <v>-1.2180629628201398E-3</v>
       </c>
       <c r="G11">
+        <v>1.2048822111075103E-2</v>
+      </c>
+      <c r="H11">
         <v>8.3432692270468851E-4</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>2.1888593728654135E-2</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>-4.8190179695063891E-4</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>-8.1010104598913039E-6</v>
-      </c>
-      <c r="K11">
-        <v>1.2048822111075103E-2</v>
       </c>
       <c r="L11">
         <v>0.16525433227324995</v>
@@ -3927,20 +3489,17 @@
         <v>-1.7327106563189906E-3</v>
       </c>
       <c r="R11">
-        <v>1.2048822111074678E-2</v>
+        <v>0.21065994568645538</v>
       </c>
       <c r="S11">
-        <v>0.21065994568645538</v>
-      </c>
-      <c r="T11">
         <v>-0.30516999809886958</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="68">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12">
         <v>-29.935741735240395</v>
       </c>
       <c r="C12">
@@ -3956,19 +3515,19 @@
         <v>-8.0500751965215112E-3</v>
       </c>
       <c r="G12">
+        <v>-6.8483072996334715E-2</v>
+      </c>
+      <c r="H12">
         <v>-6.9385984347325624E-2</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>-2.2853612385423787</v>
       </c>
-      <c r="I12">
+      <c r="J12">
         <v>5.3741914882832531E-2</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>6.9902796488167718E-2</v>
-      </c>
-      <c r="K12">
-        <v>-6.8483072996334715E-2</v>
       </c>
       <c r="L12">
         <v>-0.22780330729515086</v>
@@ -3989,20 +3548,17 @@
         <v>-2.9952192220673801E-2</v>
       </c>
       <c r="R12">
-        <v>-6.8483072997034711E-2</v>
+        <v>-1.1195151023239589</v>
       </c>
       <c r="S12">
-        <v>-1.1195151023239589</v>
-      </c>
-      <c r="T12">
         <v>38.291921533261075</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="69">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
         <v>-0.93153622381178247</v>
       </c>
       <c r="C13">
@@ -4018,19 +3574,19 @@
         <v>-1.5770525803583939E-4</v>
       </c>
       <c r="G13">
+        <v>3.1804823520365563E-4</v>
+      </c>
+      <c r="H13">
         <v>2.0875792007095254E-3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>2.5542802199271519E-4</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>-1.0167460514225873E-5</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>-1.0890264547783091E-3</v>
-      </c>
-      <c r="K13">
-        <v>3.1804823520365563E-4</v>
       </c>
       <c r="L13">
         <v>-2.3698549281644943E-3</v>
@@ -4051,20 +3607,17 @@
         <v>2.823826576787411E-3</v>
       </c>
       <c r="R13">
-        <v>3.1804823520732717E-4</v>
+        <v>4.3865715736399191E-4</v>
       </c>
       <c r="S13">
-        <v>4.3865715736399191E-4</v>
-      </c>
-      <c r="T13">
         <v>-0.20305799573377925</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="88" t="s">
-        <v>32</v>
-      </c>
-      <c r="B14" s="70">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
         <v>-0.31600492205094965</v>
       </c>
       <c r="C14">
@@ -4080,19 +3633,19 @@
         <v>-2.1803156558907189E-3</v>
       </c>
       <c r="G14">
+        <v>6.6612731888889276E-3</v>
+      </c>
+      <c r="H14">
         <v>7.6436418682022111E-3</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>0.34900827040695148</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>-8.7009815503651111E-3</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>-1.4468652241800294E-2</v>
-      </c>
-      <c r="K14">
-        <v>6.6612731888889276E-3</v>
       </c>
       <c r="L14">
         <v>2.8157907757965173E-2</v>
@@ -4113,20 +3666,17 @@
         <v>1.4483592867328587E-2</v>
       </c>
       <c r="R14">
-        <v>6.6612731888761045E-3</v>
+        <v>0.57903884826754037</v>
       </c>
       <c r="S14">
-        <v>0.57903884826754037</v>
-      </c>
-      <c r="T14">
         <v>-15.67082993210812</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="89" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="71">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15">
         <v>2.4424163226648508E-2</v>
       </c>
       <c r="C15">
@@ -4142,19 +3692,19 @@
         <v>4.6831022305089199E-5</v>
       </c>
       <c r="G15">
+        <v>-1.1980635301275539E-4</v>
+      </c>
+      <c r="H15">
         <v>-1.7606722060131089E-4</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>-7.7847833132934641E-3</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>1.9419292552027689E-4</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>3.1697426898209086E-4</v>
-      </c>
-      <c r="K15">
-        <v>-1.1980635301275539E-4</v>
       </c>
       <c r="L15">
         <v>-6.0886302818480113E-4</v>
@@ -4175,20 +3725,17 @@
         <v>-3.0131560831524878E-4</v>
       </c>
       <c r="R15">
-        <v>-1.1980635301460721E-4</v>
+        <v>-1.250599839420391E-2</v>
       </c>
       <c r="S15">
-        <v>-1.250599839420391E-2</v>
-      </c>
-      <c r="T15">
         <v>0.3440460278111015</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="90" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="72">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16">
         <v>0.21891049279469843</v>
       </c>
       <c r="C16">
@@ -4204,19 +3751,19 @@
         <v>-4.192765687167704E-5</v>
       </c>
       <c r="G16">
+        <v>1.4408950208657876E-3</v>
+      </c>
+      <c r="H16">
         <v>-5.0749219320046779E-4</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>2.4333200146942624E-3</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>-6.8682784559759638E-5</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>1.2012384574993356E-2</v>
-      </c>
-      <c r="K16">
-        <v>1.4408950208657876E-3</v>
       </c>
       <c r="L16">
         <v>-1.7327106563189906E-3</v>
@@ -4237,198 +3784,127 @@
         <v>4.4931074372669792E-2</v>
       </c>
       <c r="R16">
-        <v>1.4408950208655465E-3</v>
+        <v>-8.5272147452858486E-3</v>
       </c>
       <c r="S16">
+        <v>-0.18846867614259799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17">
+        <v>2.5221588750927721</v>
+      </c>
+      <c r="C17">
+        <v>2.2233406111747426E-3</v>
+      </c>
+      <c r="D17">
+        <v>-7.5774829137869679E-3</v>
+      </c>
+      <c r="E17">
+        <v>-1.0734460577005167E-3</v>
+      </c>
+      <c r="F17">
+        <v>-2.9275421706408105E-3</v>
+      </c>
+      <c r="G17">
+        <v>1.3892230893192671E-2</v>
+      </c>
+      <c r="H17">
+        <v>-3.0264532465248267E-3</v>
+      </c>
+      <c r="I17">
+        <v>0.11744784111344853</v>
+      </c>
+      <c r="J17">
+        <v>-2.9384538952128628E-3</v>
+      </c>
+      <c r="K17">
+        <v>1.3457265497723823E-3</v>
+      </c>
+      <c r="L17">
+        <v>0.21065994568645538</v>
+      </c>
+      <c r="M17">
+        <v>-1.1195151023239589</v>
+      </c>
+      <c r="N17">
+        <v>4.3865715736399191E-4</v>
+      </c>
+      <c r="O17">
+        <v>0.57903884826754037</v>
+      </c>
+      <c r="P17">
+        <v>-1.250599839420391E-2</v>
+      </c>
+      <c r="Q17">
         <v>-8.5272147452858486E-3</v>
       </c>
-      <c r="T16">
+      <c r="R17">
+        <v>1.1337847049663692</v>
+      </c>
+      <c r="S17">
+        <v>-6.6166349876964148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18">
+        <v>-5.7631066522682266</v>
+      </c>
+      <c r="C18">
+        <v>0.13936901697517656</v>
+      </c>
+      <c r="D18">
+        <v>0.22634927920258352</v>
+      </c>
+      <c r="E18">
+        <v>0.27644900393323169</v>
+      </c>
+      <c r="F18">
+        <v>2.1657007298017561E-2</v>
+      </c>
+      <c r="G18">
+        <v>-7.6393196346831616E-2</v>
+      </c>
+      <c r="H18">
+        <v>-8.1502980435032235E-2</v>
+      </c>
+      <c r="I18">
+        <v>-3.8831443961643544</v>
+      </c>
+      <c r="J18">
+        <v>9.6725413434437524E-2</v>
+      </c>
+      <c r="K18">
+        <v>0.15531469348685284</v>
+      </c>
+      <c r="L18">
+        <v>-0.30516999809886958</v>
+      </c>
+      <c r="M18">
+        <v>38.291921533261075</v>
+      </c>
+      <c r="N18">
+        <v>-0.20305799573377925</v>
+      </c>
+      <c r="O18">
+        <v>-15.67082993210812</v>
+      </c>
+      <c r="P18">
+        <v>0.3440460278111015</v>
+      </c>
+      <c r="Q18">
         <v>-0.18846867614259799</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="91" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="73">
-        <v>-1.2073265405911595</v>
-      </c>
-      <c r="C17">
-        <v>-5.5324896085405637E-4</v>
-      </c>
-      <c r="D17">
-        <v>8.7304371488505599E-4</v>
-      </c>
-      <c r="E17">
-        <v>4.6451815529675086E-4</v>
-      </c>
-      <c r="F17">
-        <v>-9.5629351866939605E-4</v>
-      </c>
-      <c r="G17">
-        <v>-2.9223241728486274E-3</v>
-      </c>
-      <c r="H17">
-        <v>5.7739783668786515E-3</v>
-      </c>
-      <c r="I17">
-        <v>-8.3991358960842227E-5</v>
-      </c>
-      <c r="J17">
-        <v>3.0891323863097963E-3</v>
-      </c>
-      <c r="K17">
-        <v>6.0474412373201447E-2</v>
-      </c>
-      <c r="L17">
-        <v>1.2048822111074678E-2</v>
-      </c>
-      <c r="M17">
-        <v>-6.8483072997034711E-2</v>
-      </c>
-      <c r="N17">
-        <v>3.1804823520732717E-4</v>
-      </c>
-      <c r="O17">
-        <v>6.6612731888761045E-3</v>
-      </c>
-      <c r="P17">
-        <v>-1.1980635301460721E-4</v>
-      </c>
-      <c r="Q17">
-        <v>1.4408950208655465E-3</v>
-      </c>
-      <c r="R17">
-        <v>6.0474412373201461E-2</v>
-      </c>
-      <c r="S17">
-        <v>1.3892230893192671E-2</v>
-      </c>
-      <c r="T17">
-        <v>-7.639319634683206E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="92" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="74">
-        <v>2.5221588750927721</v>
-      </c>
-      <c r="C18">
-        <v>2.2233406111747426E-3</v>
-      </c>
-      <c r="D18">
-        <v>-7.5774829137869679E-3</v>
-      </c>
-      <c r="E18">
-        <v>-1.0734460577005167E-3</v>
-      </c>
-      <c r="F18">
-        <v>-2.9275421706408105E-3</v>
-      </c>
-      <c r="G18">
-        <v>-3.0264532465248267E-3</v>
-      </c>
-      <c r="H18">
-        <v>0.11744784111344853</v>
-      </c>
-      <c r="I18">
-        <v>-2.9384538952128628E-3</v>
-      </c>
-      <c r="J18">
-        <v>1.3457265497723823E-3</v>
-      </c>
-      <c r="K18">
-        <v>1.3892230893192671E-2</v>
-      </c>
-      <c r="L18">
-        <v>0.21065994568645538</v>
-      </c>
-      <c r="M18">
-        <v>-1.1195151023239589</v>
-      </c>
-      <c r="N18">
-        <v>4.3865715736399191E-4</v>
-      </c>
-      <c r="O18">
-        <v>0.57903884826754037</v>
-      </c>
-      <c r="P18">
-        <v>-1.250599839420391E-2</v>
-      </c>
-      <c r="Q18">
-        <v>-8.5272147452858486E-3</v>
-      </c>
       <c r="R18">
-        <v>1.3892230893192671E-2</v>
+        <v>-6.6166349876964148</v>
       </c>
       <c r="S18">
-        <v>1.1337847049663692</v>
-      </c>
-      <c r="T18">
-        <v>-6.6166349876964148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="93" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="75">
-        <v>-5.7631066522682266</v>
-      </c>
-      <c r="C19">
-        <v>0.13936901697517656</v>
-      </c>
-      <c r="D19">
-        <v>0.22634927920258352</v>
-      </c>
-      <c r="E19">
-        <v>0.27644900393323169</v>
-      </c>
-      <c r="F19">
-        <v>2.1657007298017561E-2</v>
-      </c>
-      <c r="G19">
-        <v>-8.1502980435032235E-2</v>
-      </c>
-      <c r="H19">
-        <v>-3.8831443961643544</v>
-      </c>
-      <c r="I19">
-        <v>9.6725413434437524E-2</v>
-      </c>
-      <c r="J19">
-        <v>0.15531469348685284</v>
-      </c>
-      <c r="K19">
-        <v>-7.6393196346831616E-2</v>
-      </c>
-      <c r="L19">
-        <v>-0.30516999809886958</v>
-      </c>
-      <c r="M19">
-        <v>38.291921533261075</v>
-      </c>
-      <c r="N19">
-        <v>-0.20305799573377925</v>
-      </c>
-      <c r="O19">
-        <v>-15.67082993210812</v>
-      </c>
-      <c r="P19">
-        <v>0.3440460278111015</v>
-      </c>
-      <c r="Q19">
-        <v>-0.18846867614259799</v>
-      </c>
-      <c r="R19">
-        <v>-7.639319634683206E-2</v>
-      </c>
-      <c r="S19">
-        <v>-6.6166349876964148</v>
-      </c>
-      <c r="T19">
         <v>176.8290461332399</v>
       </c>
     </row>

</xml_diff>